<commit_message>
Added in real values for inflation and exported figures
</commit_message>
<xml_diff>
--- a/data/clean_data/milk_df_clean.xlsx
+++ b/data/clean_data/milk_df_clean.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,30 +466,55 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>vet_costs</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>bedding_litter_costs</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>marketing_costs</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>operating_costs</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>service_costs</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>utility_costs</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>repair_costs</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>total_operating_costs</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>overhead</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>total_costs</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>cows_per_farm</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>output_per_cow</t>
         </is>
@@ -519,21 +544,36 @@
         <v>10.11</v>
       </c>
       <c r="G2" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="I2" t="n">
         <v>0.43</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="M2" t="n">
         <v>14.3</v>
       </c>
-      <c r="I2" t="n">
+      <c r="N2" t="n">
         <v>16.31</v>
       </c>
-      <c r="J2" t="n">
+      <c r="O2" t="n">
         <v>30.61</v>
       </c>
-      <c r="K2" t="n">
+      <c r="P2" t="n">
         <v>59</v>
       </c>
-      <c r="L2" t="n">
+      <c r="Q2" t="n">
         <v>13058</v>
       </c>
     </row>
@@ -561,21 +601,36 @@
         <v>13.08</v>
       </c>
       <c r="G3" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="I3" t="n">
         <v>0.24</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="M3" t="n">
         <v>16.63</v>
       </c>
-      <c r="I3" t="n">
+      <c r="N3" t="n">
         <v>21.37</v>
       </c>
-      <c r="J3" t="n">
+      <c r="O3" t="n">
         <v>38</v>
       </c>
-      <c r="K3" t="n">
+      <c r="P3" t="n">
         <v>53</v>
       </c>
-      <c r="L3" t="n">
+      <c r="Q3" t="n">
         <v>10956</v>
       </c>
     </row>
@@ -603,21 +658,36 @@
         <v>13.23</v>
       </c>
       <c r="G4" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="I4" t="n">
         <v>0.31</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="M4" t="n">
         <v>17.1</v>
       </c>
-      <c r="I4" t="n">
+      <c r="N4" t="n">
         <v>14.61</v>
       </c>
-      <c r="J4" t="n">
+      <c r="O4" t="n">
         <v>31.71</v>
       </c>
-      <c r="K4" t="n">
+      <c r="P4" t="n">
         <v>46</v>
       </c>
-      <c r="L4" t="n">
+      <c r="Q4" t="n">
         <v>12177</v>
       </c>
     </row>
@@ -645,21 +715,36 @@
         <v>13.61</v>
       </c>
       <c r="G5" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.24</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="M5" t="n">
         <v>17.62</v>
       </c>
-      <c r="I5" t="n">
+      <c r="N5" t="n">
         <v>18.88</v>
       </c>
-      <c r="J5" t="n">
+      <c r="O5" t="n">
         <v>36.5</v>
       </c>
-      <c r="K5" t="n">
+      <c r="P5" t="n">
         <v>62</v>
       </c>
-      <c r="L5" t="n">
+      <c r="Q5" t="n">
         <v>11982</v>
       </c>
     </row>
@@ -687,21 +772,36 @@
         <v>13.47</v>
       </c>
       <c r="G6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="I6" t="n">
         <v>0.22</v>
       </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="M6" t="n">
         <v>17.11</v>
       </c>
-      <c r="I6" t="n">
+      <c r="N6" t="n">
         <v>14.95</v>
       </c>
-      <c r="J6" t="n">
+      <c r="O6" t="n">
         <v>32.07</v>
       </c>
-      <c r="K6" t="n">
+      <c r="P6" t="n">
         <v>65</v>
       </c>
-      <c r="L6" t="n">
+      <c r="Q6" t="n">
         <v>13101</v>
       </c>
     </row>
@@ -729,21 +829,36 @@
         <v>14.01</v>
       </c>
       <c r="G7" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.25</v>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="M7" t="n">
         <v>17.89</v>
       </c>
-      <c r="I7" t="n">
+      <c r="N7" t="n">
         <v>21.99</v>
       </c>
-      <c r="J7" t="n">
+      <c r="O7" t="n">
         <v>39.88</v>
       </c>
-      <c r="K7" t="n">
+      <c r="P7" t="n">
         <v>36</v>
       </c>
-      <c r="L7" t="n">
+      <c r="Q7" t="n">
         <v>10542</v>
       </c>
     </row>
@@ -771,21 +886,36 @@
         <v>11.58</v>
       </c>
       <c r="G8" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="I8" t="n">
         <v>0.39</v>
       </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="M8" t="n">
         <v>16.39</v>
       </c>
-      <c r="I8" t="n">
+      <c r="N8" t="n">
         <v>18.1</v>
       </c>
-      <c r="J8" t="n">
+      <c r="O8" t="n">
         <v>34.48999999999999</v>
       </c>
-      <c r="K8" t="n">
+      <c r="P8" t="n">
         <v>73</v>
       </c>
-      <c r="L8" t="n">
+      <c r="Q8" t="n">
         <v>12880</v>
       </c>
     </row>
@@ -813,21 +943,36 @@
         <v>14.05</v>
       </c>
       <c r="G9" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="I9" t="n">
         <v>0.23</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="M9" t="n">
         <v>18.81</v>
       </c>
-      <c r="I9" t="n">
+      <c r="N9" t="n">
         <v>20.52</v>
       </c>
-      <c r="J9" t="n">
+      <c r="O9" t="n">
         <v>39.33</v>
       </c>
-      <c r="K9" t="n">
+      <c r="P9" t="n">
         <v>72</v>
       </c>
-      <c r="L9" t="n">
+      <c r="Q9" t="n">
         <v>12247</v>
       </c>
     </row>
@@ -855,21 +1000,36 @@
         <v>15.88</v>
       </c>
       <c r="G10" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I10" t="n">
         <v>0.23</v>
       </c>
-      <c r="H10" t="n">
+      <c r="J10" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="M10" t="n">
         <v>21.05</v>
       </c>
-      <c r="I10" t="n">
+      <c r="N10" t="n">
         <v>22.45</v>
       </c>
-      <c r="J10" t="n">
+      <c r="O10" t="n">
         <v>43.5</v>
       </c>
-      <c r="K10" t="n">
+      <c r="P10" t="n">
         <v>60</v>
       </c>
-      <c r="L10" t="n">
+      <c r="Q10" t="n">
         <v>12145</v>
       </c>
     </row>
@@ -897,21 +1057,36 @@
         <v>14.75</v>
       </c>
       <c r="G11" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="I11" t="n">
         <v>0.19</v>
       </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="M11" t="n">
         <v>19.85</v>
       </c>
-      <c r="I11" t="n">
+      <c r="N11" t="n">
         <v>21.15</v>
       </c>
-      <c r="J11" t="n">
+      <c r="O11" t="n">
         <v>41</v>
       </c>
-      <c r="K11" t="n">
+      <c r="P11" t="n">
         <v>56</v>
       </c>
-      <c r="L11" t="n">
+      <c r="Q11" t="n">
         <v>12940</v>
       </c>
     </row>
@@ -939,21 +1114,36 @@
         <v>12.93</v>
       </c>
       <c r="G12" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="I12" t="n">
         <v>0.2</v>
       </c>
-      <c r="H12" t="n">
+      <c r="J12" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="L12" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="M12" t="n">
         <v>18.56</v>
       </c>
-      <c r="I12" t="n">
+      <c r="N12" t="n">
         <v>16.47</v>
       </c>
-      <c r="J12" t="n">
+      <c r="O12" t="n">
         <v>35.03</v>
       </c>
-      <c r="K12" t="n">
+      <c r="P12" t="n">
         <v>89</v>
       </c>
-      <c r="L12" t="n">
+      <c r="Q12" t="n">
         <v>13376</v>
       </c>
     </row>
@@ -981,21 +1171,36 @@
         <v>23.65</v>
       </c>
       <c r="G13" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="I13" t="n">
         <v>0.1</v>
       </c>
-      <c r="H13" t="n">
+      <c r="J13" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="M13" t="n">
         <v>28.56000000000001</v>
       </c>
-      <c r="I13" t="n">
+      <c r="N13" t="n">
         <v>18.06</v>
       </c>
-      <c r="J13" t="n">
+      <c r="O13" t="n">
         <v>46.62</v>
       </c>
-      <c r="K13" t="n">
+      <c r="P13" t="n">
         <v>62</v>
       </c>
-      <c r="L13" t="n">
+      <c r="Q13" t="n">
         <v>12223</v>
       </c>
     </row>
@@ -1023,21 +1228,36 @@
         <v>13.12</v>
       </c>
       <c r="G14" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="I14" t="n">
         <v>0.22</v>
       </c>
-      <c r="H14" t="n">
+      <c r="J14" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="M14" t="n">
         <v>17.51</v>
       </c>
-      <c r="I14" t="n">
+      <c r="N14" t="n">
         <v>20.35</v>
       </c>
-      <c r="J14" t="n">
+      <c r="O14" t="n">
         <v>37.86</v>
       </c>
-      <c r="K14" t="n">
+      <c r="P14" t="n">
         <v>37</v>
       </c>
-      <c r="L14" t="n">
+      <c r="Q14" t="n">
         <v>13178</v>
       </c>
     </row>
@@ -1065,21 +1285,36 @@
         <v>15.91</v>
       </c>
       <c r="G15" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="H15" t="n">
         <v>0.25</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="M15" t="n">
         <v>20</v>
       </c>
-      <c r="I15" t="n">
+      <c r="N15" t="n">
         <v>17.58</v>
       </c>
-      <c r="J15" t="n">
+      <c r="O15" t="n">
         <v>37.58</v>
       </c>
-      <c r="K15" t="n">
+      <c r="P15" t="n">
         <v>49</v>
       </c>
-      <c r="L15" t="n">
+      <c r="Q15" t="n">
         <v>14543</v>
       </c>
     </row>
@@ -1107,21 +1342,36 @@
         <v>15.52</v>
       </c>
       <c r="G16" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="I16" t="n">
         <v>0.37</v>
       </c>
-      <c r="H16" t="n">
+      <c r="J16" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="L16" t="n">
+        <v>3.02</v>
+      </c>
+      <c r="M16" t="n">
         <v>22.64</v>
       </c>
-      <c r="I16" t="n">
+      <c r="N16" t="n">
         <v>18.17</v>
       </c>
-      <c r="J16" t="n">
+      <c r="O16" t="n">
         <v>40.81</v>
       </c>
-      <c r="K16" t="n">
+      <c r="P16" t="n">
         <v>63</v>
       </c>
-      <c r="L16" t="n">
+      <c r="Q16" t="n">
         <v>14211</v>
       </c>
     </row>
@@ -1149,21 +1399,36 @@
         <v>8.159999999999998</v>
       </c>
       <c r="G17" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="I17" t="n">
         <v>0.28</v>
       </c>
-      <c r="H17" t="n">
+      <c r="J17" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="M17" t="n">
         <v>10.24</v>
       </c>
-      <c r="I17" t="n">
+      <c r="N17" t="n">
         <v>3.88</v>
       </c>
-      <c r="J17" t="n">
+      <c r="O17" t="n">
         <v>14.12</v>
       </c>
-      <c r="K17" t="n">
+      <c r="P17" t="n">
         <v>988</v>
       </c>
-      <c r="L17" t="n">
+      <c r="Q17" t="n">
         <v>19987</v>
       </c>
     </row>
@@ -1191,21 +1456,36 @@
         <v>9.06</v>
       </c>
       <c r="G18" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I18" t="n">
         <v>0.18</v>
       </c>
-      <c r="H18" t="n">
+      <c r="J18" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="M18" t="n">
         <v>12.42</v>
       </c>
-      <c r="I18" t="n">
+      <c r="N18" t="n">
         <v>6.42</v>
       </c>
-      <c r="J18" t="n">
+      <c r="O18" t="n">
         <v>18.84</v>
       </c>
-      <c r="K18" t="n">
+      <c r="P18" t="n">
         <v>1013</v>
       </c>
-      <c r="L18" t="n">
+      <c r="Q18" t="n">
         <v>17572</v>
       </c>
     </row>
@@ -1233,21 +1513,36 @@
         <v>7.590000000000001</v>
       </c>
       <c r="G19" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I19" t="n">
         <v>0.7</v>
       </c>
-      <c r="H19" t="n">
+      <c r="J19" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="M19" t="n">
         <v>11.06</v>
       </c>
-      <c r="I19" t="n">
+      <c r="N19" t="n">
         <v>7.419999999999999</v>
       </c>
-      <c r="J19" t="n">
+      <c r="O19" t="n">
         <v>18.48</v>
       </c>
-      <c r="K19" t="n">
+      <c r="P19" t="n">
         <v>273</v>
       </c>
-      <c r="L19" t="n">
+      <c r="Q19" t="n">
         <v>17294</v>
       </c>
     </row>
@@ -1275,21 +1570,36 @@
         <v>8.91</v>
       </c>
       <c r="G20" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="I20" t="n">
         <v>0.25</v>
       </c>
-      <c r="H20" t="n">
+      <c r="J20" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="M20" t="n">
         <v>11.93</v>
       </c>
-      <c r="I20" t="n">
+      <c r="N20" t="n">
         <v>9.010000000000002</v>
       </c>
-      <c r="J20" t="n">
+      <c r="O20" t="n">
         <v>20.94</v>
       </c>
-      <c r="K20" t="n">
+      <c r="P20" t="n">
         <v>133</v>
       </c>
-      <c r="L20" t="n">
+      <c r="Q20" t="n">
         <v>17949</v>
       </c>
     </row>
@@ -1317,21 +1627,36 @@
         <v>7.579999999999999</v>
       </c>
       <c r="G21" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="I21" t="n">
         <v>0.29</v>
       </c>
-      <c r="H21" t="n">
+      <c r="J21" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="M21" t="n">
         <v>11.23</v>
       </c>
-      <c r="I21" t="n">
+      <c r="N21" t="n">
         <v>9.57</v>
       </c>
-      <c r="J21" t="n">
+      <c r="O21" t="n">
         <v>20.8</v>
       </c>
-      <c r="K21" t="n">
+      <c r="P21" t="n">
         <v>127</v>
       </c>
-      <c r="L21" t="n">
+      <c r="Q21" t="n">
         <v>18389</v>
       </c>
     </row>
@@ -1359,21 +1684,36 @@
         <v>9.210000000000001</v>
       </c>
       <c r="G22" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="I22" t="n">
         <v>0.28</v>
       </c>
-      <c r="H22" t="n">
+      <c r="J22" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="M22" t="n">
         <v>11.46</v>
       </c>
-      <c r="I22" t="n">
+      <c r="N22" t="n">
         <v>4.56</v>
       </c>
-      <c r="J22" t="n">
+      <c r="O22" t="n">
         <v>16.02</v>
       </c>
-      <c r="K22" t="n">
+      <c r="P22" t="n">
         <v>999</v>
       </c>
-      <c r="L22" t="n">
+      <c r="Q22" t="n">
         <v>22569</v>
       </c>
     </row>
@@ -1401,21 +1741,36 @@
         <v>11.69</v>
       </c>
       <c r="G23" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I23" t="n">
         <v>0.15</v>
       </c>
-      <c r="H23" t="n">
+      <c r="J23" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="M23" t="n">
         <v>14.25</v>
       </c>
-      <c r="I23" t="n">
+      <c r="N23" t="n">
         <v>8.200000000000001</v>
       </c>
-      <c r="J23" t="n">
+      <c r="O23" t="n">
         <v>22.45</v>
       </c>
-      <c r="K23" t="n">
+      <c r="P23" t="n">
         <v>905</v>
       </c>
-      <c r="L23" t="n">
+      <c r="Q23" t="n">
         <v>18071</v>
       </c>
     </row>
@@ -1443,21 +1798,36 @@
         <v>9.789999999999999</v>
       </c>
       <c r="G24" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="I24" t="n">
         <v>0.2</v>
       </c>
-      <c r="H24" t="n">
+      <c r="J24" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="M24" t="n">
         <v>12.65</v>
       </c>
-      <c r="I24" t="n">
+      <c r="N24" t="n">
         <v>9.869999999999999</v>
       </c>
-      <c r="J24" t="n">
+      <c r="O24" t="n">
         <v>22.52</v>
       </c>
-      <c r="K24" t="n">
+      <c r="P24" t="n">
         <v>188</v>
       </c>
-      <c r="L24" t="n">
+      <c r="Q24" t="n">
         <v>15518</v>
       </c>
     </row>
@@ -1485,21 +1855,36 @@
         <v>8.130000000000001</v>
       </c>
       <c r="G25" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="I25" t="n">
         <v>0.26</v>
       </c>
-      <c r="H25" t="n">
+      <c r="J25" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="M25" t="n">
         <v>10.14</v>
       </c>
-      <c r="I25" t="n">
+      <c r="N25" t="n">
         <v>3.36</v>
       </c>
-      <c r="J25" t="n">
+      <c r="O25" t="n">
         <v>13.5</v>
       </c>
-      <c r="K25" t="n">
+      <c r="P25" t="n">
         <v>1110</v>
       </c>
-      <c r="L25" t="n">
+      <c r="Q25" t="n">
         <v>22085</v>
       </c>
     </row>
@@ -1527,21 +1912,36 @@
         <v>10.64</v>
       </c>
       <c r="G26" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="I26" t="n">
         <v>0.18</v>
       </c>
-      <c r="H26" t="n">
+      <c r="J26" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="M26" t="n">
         <v>14.76</v>
       </c>
-      <c r="I26" t="n">
+      <c r="N26" t="n">
         <v>13.1</v>
       </c>
-      <c r="J26" t="n">
+      <c r="O26" t="n">
         <v>27.86</v>
       </c>
-      <c r="K26" t="n">
+      <c r="P26" t="n">
         <v>80</v>
       </c>
-      <c r="L26" t="n">
+      <c r="Q26" t="n">
         <v>18082</v>
       </c>
     </row>
@@ -1569,21 +1969,36 @@
         <v>8.859999999999999</v>
       </c>
       <c r="G27" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="I27" t="n">
         <v>0.24</v>
       </c>
-      <c r="H27" t="n">
+      <c r="J27" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M27" t="n">
         <v>11.22</v>
       </c>
-      <c r="I27" t="n">
+      <c r="N27" t="n">
         <v>5.659999999999999</v>
       </c>
-      <c r="J27" t="n">
+      <c r="O27" t="n">
         <v>16.88</v>
       </c>
-      <c r="K27" t="n">
+      <c r="P27" t="n">
         <v>1746</v>
       </c>
-      <c r="L27" t="n">
+      <c r="Q27" t="n">
         <v>21703</v>
       </c>
     </row>
@@ -1611,21 +2026,36 @@
         <v>11.28</v>
       </c>
       <c r="G28" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="I28" t="n">
         <v>0.14</v>
       </c>
-      <c r="H28" t="n">
+      <c r="J28" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="M28" t="n">
         <v>15.85</v>
       </c>
-      <c r="I28" t="n">
+      <c r="N28" t="n">
         <v>9.470000000000001</v>
       </c>
-      <c r="J28" t="n">
+      <c r="O28" t="n">
         <v>25.32</v>
       </c>
-      <c r="K28" t="n">
+      <c r="P28" t="n">
         <v>177</v>
       </c>
-      <c r="L28" t="n">
+      <c r="Q28" t="n">
         <v>20068</v>
       </c>
     </row>
@@ -1653,21 +2083,36 @@
         <v>9.970000000000001</v>
       </c>
       <c r="G29" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="I29" t="n">
         <v>0.12</v>
       </c>
-      <c r="H29" t="n">
+      <c r="J29" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="M29" t="n">
         <v>13.47</v>
       </c>
-      <c r="I29" t="n">
+      <c r="N29" t="n">
         <v>8.85</v>
       </c>
-      <c r="J29" t="n">
+      <c r="O29" t="n">
         <v>22.32</v>
       </c>
-      <c r="K29" t="n">
+      <c r="P29" t="n">
         <v>144</v>
       </c>
-      <c r="L29" t="n">
+      <c r="Q29" t="n">
         <v>20920</v>
       </c>
     </row>
@@ -1695,21 +2140,36 @@
         <v>8.619999999999999</v>
       </c>
       <c r="G30" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="I30" t="n">
         <v>0.13</v>
       </c>
-      <c r="H30" t="n">
+      <c r="J30" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="M30" t="n">
         <v>11.82</v>
       </c>
-      <c r="I30" t="n">
+      <c r="N30" t="n">
         <v>8.300000000000001</v>
       </c>
-      <c r="J30" t="n">
+      <c r="O30" t="n">
         <v>20.12</v>
       </c>
-      <c r="K30" t="n">
+      <c r="P30" t="n">
         <v>246</v>
       </c>
-      <c r="L30" t="n">
+      <c r="Q30" t="n">
         <v>23086</v>
       </c>
     </row>
@@ -1737,21 +2197,36 @@
         <v>9.589999999999998</v>
       </c>
       <c r="G31" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="I31" t="n">
         <v>0.18</v>
       </c>
-      <c r="H31" t="n">
+      <c r="J31" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="M31" t="n">
         <v>12.77</v>
       </c>
-      <c r="I31" t="n">
+      <c r="N31" t="n">
         <v>7.989999999999999</v>
       </c>
-      <c r="J31" t="n">
+      <c r="O31" t="n">
         <v>20.75999999999999</v>
       </c>
-      <c r="K31" t="n">
+      <c r="P31" t="n">
         <v>139</v>
       </c>
-      <c r="L31" t="n">
+      <c r="Q31" t="n">
         <v>19561</v>
       </c>
     </row>

</xml_diff>